<commit_message>
Understood the criticality of Excel's stable sort to the algorithm
</commit_message>
<xml_diff>
--- a/Excel_Challenge_607 - Sort Odd Numbers First.xlsx
+++ b/Excel_Challenge_607 - Sort Odd Numbers First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392310E-6B81-4D3E-A42C-82F6BF0C75C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F102768-FB17-4299-9FF8-E96BD4B56985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/excelbi/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>Uses the stability of the Excel Sort. Important observations.</t>
   </si>
 </sst>
 </file>
@@ -611,6 +614,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1349,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072A9761-4FA0-4541-8C6C-23058228B328}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,6 +1612,9 @@
       </c>
       <c r="E16">
         <v>92</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>